<commit_message>
Added Updated Board and BOM, note this will not be the final revision
</commit_message>
<xml_diff>
--- a/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
+++ b/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
   <si>
     <t xml:space="preserve">Bill of materials for Group 3, Voice Recognition Project</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ext. Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">PWR-BLU</t>
@@ -371,7 +374,58 @@
     <t xml:space="preserve">TOL-12889</t>
   </si>
   <si>
-    <t xml:space="preserve">Ver # 1</t>
+    <t xml:space="preserve">USB-A Cable 2 pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB-A Male to Male 4ft cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actually 8.20 per 2 pk but only cost 4.1 per board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 Pack cables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elegoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ml to Ml, Fm to Ml, Fm to Fm Connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only 1 bundled need for all 4 boards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misc Connectors EPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPL-PSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous Headers from EPL Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISC EPL Fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reflow fees, soldering fees, etc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Total Cost:</t>
@@ -387,7 +441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -442,6 +496,18 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -491,7 +557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -558,6 +624,14 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -649,26 +723,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4285714285714"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.780612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10714285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4387755102041"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.3826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.3724489795918"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6836734693878"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3928571428571"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9234693877551"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,6 +913,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="ALX7" s="0"/>
       <c r="ALY7" s="0"/>
       <c r="ALZ7" s="0"/>
@@ -864,6 +940,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="ALX8" s="0"/>
       <c r="ALY8" s="0"/>
       <c r="ALZ8" s="0"/>
@@ -912,6 +989,9 @@
       <c r="K9" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="L9" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="ALX9" s="0"/>
       <c r="ALY9" s="0"/>
       <c r="ALZ9" s="0"/>
@@ -931,28 +1011,28 @@
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J10" s="12" t="n">
         <v>0.9</v>
@@ -967,28 +1047,28 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J11" s="13" t="n">
         <v>0.51</v>
@@ -1003,28 +1083,28 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J12" s="12" t="n">
         <v>0.72</v>
@@ -1039,28 +1119,28 @@
         <v>1</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J13" s="12" t="n">
         <v>0.72</v>
@@ -1075,28 +1155,28 @@
         <v>2</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>0.3</v>
@@ -1108,38 +1188,38 @@
     </row>
     <row r="15" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J15" s="12" t="n">
         <v>0.71</v>
       </c>
       <c r="K15" s="10" t="n">
         <f aca="false">A15*J15</f>
-        <v>2.84</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1147,28 +1227,28 @@
         <v>2</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J16" s="12" t="n">
         <v>0.59</v>
@@ -1180,38 +1260,38 @@
     </row>
     <row r="17" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J17" s="12" t="n">
         <v>0.94</v>
       </c>
       <c r="K17" s="10" t="n">
         <f aca="false">A17*J17</f>
-        <v>1.88</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,28 +1299,28 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J18" s="12" t="n">
         <v>0.92</v>
@@ -1255,28 +1335,28 @@
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J19" s="12" t="n">
         <v>0.74</v>
@@ -1291,28 +1371,28 @@
         <v>4</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="15" t="n">
         <v>0.44</v>
@@ -1327,28 +1407,28 @@
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J21" s="12" t="n">
         <v>1.36</v>
@@ -1366,25 +1446,25 @@
         <v>22</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J22" s="12" t="n">
         <v>0.1</v>
@@ -1399,28 +1479,28 @@
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J23" s="15" t="n">
         <v>1.5</v>
@@ -1435,28 +1515,28 @@
         <v>1</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C24" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="H24" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J24" s="15" t="n">
         <v>4.12</v>
@@ -1471,28 +1551,28 @@
         <v>1</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>104</v>
-      </c>
       <c r="H25" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J25" s="12" t="n">
         <v>1.28</v>
@@ -1502,33 +1582,33 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J26" s="10" t="n">
         <v>5.95</v>
@@ -1538,40 +1618,189 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="3" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19" t="n">
-        <f aca="false">SUM(K10:K26)</f>
-        <v>27.92</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
+      <c r="C27" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+      <c r="D27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" s="10" t="n">
+        <f aca="false">8.2/2</f>
+        <v>4.1</v>
+      </c>
+      <c r="K27" s="10" t="n">
+        <f aca="false">A27*J27</f>
+        <v>4.1</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="J28" s="10" t="n">
+        <v>6.98</v>
+      </c>
+      <c r="K28" s="10" t="n">
+        <f aca="false">A28*J28</f>
+        <v>6.98</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K29" s="10" t="n">
+        <f aca="false">A29*J29</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="K30" s="10" t="n">
+        <f aca="false">A30*J30</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21" t="n">
+        <f aca="false">SUM(K10:K29)</f>
+        <v>40.35</v>
+      </c>
+      <c r="L31" s="20"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1582,9 +1811,13 @@
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A32:F32"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I27" r:id="rId1" location="" display="link"/>
+    <hyperlink ref="I28" r:id="rId2" display="link"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added a few changes to the board per andrew's suggestion
</commit_message>
<xml_diff>
--- a/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
+++ b/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
   <si>
     <t xml:space="preserve">Bill of materials for Group 3, Voice Recognition Project</t>
   </si>
@@ -392,9 +392,6 @@
     <t xml:space="preserve">link</t>
   </si>
   <si>
-    <t xml:space="preserve">Actually 8.20 per 2 pk but only cost 4.1 per board</t>
-  </si>
-  <si>
     <t xml:space="preserve">120 Pack cables</t>
   </si>
   <si>
@@ -417,12 +414,6 @@
   </si>
   <si>
     <t xml:space="preserve">EPL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISC EPL Fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reflow fees, soldering fees, etc. </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -506,7 +497,6 @@
       <sz val="11"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -723,10 +713,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:32"/>
+  <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1188,7 +1178,7 @@
     </row>
     <row r="15" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>48</v>
@@ -1219,7 +1209,7 @@
       </c>
       <c r="K15" s="10" t="n">
         <f aca="false">A15*J15</f>
-        <v>2.13</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,15 +1637,11 @@
         <v>122</v>
       </c>
       <c r="J27" s="10" t="n">
-        <f aca="false">8.2/2</f>
-        <v>4.1</v>
+        <v>8.2</v>
       </c>
       <c r="K27" s="10" t="n">
         <f aca="false">A27*J27</f>
-        <v>4.1</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>123</v>
+        <v>8.2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>111</v>
@@ -1672,13 +1658,13 @@
         <v>112</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>96</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>121</v>
@@ -1694,7 +1680,7 @@
         <v>6.98</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1702,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>111</v>
@@ -1711,16 +1697,16 @@
         <v>112</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>96</v>
       </c>
       <c r="G29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>131</v>
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="10" t="n">
@@ -1731,43 +1717,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="10" t="s">
+    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G30" s="10" t="s">
+      <c r="J30" s="21"/>
+      <c r="K30" s="21" t="n">
+        <f aca="false">SUM(K10:K29)</f>
+        <v>48</v>
+      </c>
+      <c r="L30" s="20"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="K30" s="10" t="n">
-        <f aca="false">A30*J30</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -1776,31 +1749,10 @@
       <c r="F31" s="19"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21" t="n">
-        <f aca="false">SUM(K10:K29)</f>
-        <v>40.35</v>
-      </c>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
       <c r="L31" s="20"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1811,8 +1763,8 @@
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A30:F30"/>
     <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A32:F32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I27" r:id="rId1" location="" display="link"/>

</xml_diff>

<commit_message>
Purchased the completed BOM and thus updated the transaction history on the BOM to reflect the dollars amounts contributed by each member
</commit_message>
<xml_diff>
--- a/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
+++ b/BoardDesign/VoiceRecognitionGroup3_BOM_V1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="979" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="VoiceRecognitionGroup3" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SpendingRecord" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="140">
   <si>
     <t xml:space="preserve">Bill of materials for Group 3, Voice Recognition Project</t>
   </si>
@@ -79,7 +80,7 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">PWR-BLU</t>
+    <t xml:space="preserve">PWR-GRN</t>
   </si>
   <si>
     <t xml:space="preserve">LED1</t>
@@ -88,34 +89,28 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
-    <t xml:space="preserve">Dialight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">597-6601-607F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206 Blue LED </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">645-597-6601-607F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNC_GRN</t>
+    <t xml:space="preserve">EPL-PSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through hole Green LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNC_ORNG</t>
   </si>
   <si>
     <t xml:space="preserve">LED2</t>
   </si>
   <si>
-    <t xml:space="preserve">599-0281-007F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206 Green LED </t>
-  </si>
-  <si>
-    <t xml:space="preserve">645-599-0281-007F </t>
+    <t xml:space="preserve">Through hole Orange LED</t>
   </si>
   <si>
     <t xml:space="preserve">NOFUNC_RED</t>
@@ -124,13 +119,7 @@
     <t xml:space="preserve">LED3</t>
   </si>
   <si>
-    <t xml:space="preserve">597-6001-607F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206 Red LED </t>
-  </si>
-  <si>
-    <t xml:space="preserve">645-597-6001-607F </t>
+    <t xml:space="preserve">Through hole Red LED</t>
   </si>
   <si>
     <t xml:space="preserve">WARN_YELL</t>
@@ -139,13 +128,7 @@
     <t xml:space="preserve">LED4</t>
   </si>
   <si>
-    <t xml:space="preserve">597-6401-607F </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206 Yellow LED </t>
-  </si>
-  <si>
-    <t xml:space="preserve">645-597-6401-607F </t>
+    <t xml:space="preserve">Through hole Yellow LED</t>
   </si>
   <si>
     <t xml:space="preserve">MIC_ON, RESET1</t>
@@ -164,6 +147,9 @@
     <t xml:space="preserve">Tactile button 6mm square</t>
   </si>
   <si>
+    <t xml:space="preserve">Mouser</t>
+  </si>
+  <si>
     <t xml:space="preserve">667-EVQ-Q2K01W </t>
   </si>
   <si>
@@ -311,9 +297,6 @@
     <t xml:space="preserve">Adam Tech.</t>
   </si>
   <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
     <t xml:space="preserve">Barrel Jack Female 5.5mm jack, 2.1mm center pole diameter</t>
   </si>
   <si>
@@ -407,15 +390,9 @@
     <t xml:space="preserve">Misc Connectors EPL</t>
   </si>
   <si>
-    <t xml:space="preserve">EPL-PSU</t>
-  </si>
-  <si>
     <t xml:space="preserve">Miscellaneous Headers from EPL Store</t>
   </si>
   <si>
-    <t xml:space="preserve">EPL</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -423,16 +400,60 @@
   </si>
   <si>
     <t xml:space="preserve">Version Changes: Initial BOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Purchased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals by Purchaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototype Board, op-amp +shipping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rawan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="[$$]#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -452,6 +473,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lohit Devanagari"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -498,6 +524,17 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -522,7 +559,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -546,45 +583,40 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,34 +628,42 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -632,18 +672,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Gnumeric-default" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -715,8 +792,8 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -945,7 +1022,7 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="2" customFormat="true" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="2" customFormat="true" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1073,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
         <v>1</v>
       </c>
@@ -1025,14 +1102,14 @@
         <v>26</v>
       </c>
       <c r="J10" s="12" t="n">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
       <c r="K10" s="10" t="n">
         <f aca="false">A10*J10</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
         <v>1</v>
       </c>
@@ -1049,34 +1126,34 @@
         <v>22</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J11" s="13" t="n">
-        <v>0.51</v>
+        <v>0.25</v>
       </c>
       <c r="K11" s="10" t="n">
         <f aca="false">A11*J11</f>
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>21</v>
@@ -1085,34 +1162,34 @@
         <v>22</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="J12" s="12" t="n">
-        <v>0.72</v>
+        <v>0.25</v>
       </c>
       <c r="K12" s="10" t="n">
         <f aca="false">A12*J12</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>21</v>
@@ -1121,23 +1198,23 @@
         <v>22</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J13" s="12" t="n">
-        <v>0.72</v>
+        <v>0.25</v>
       </c>
       <c r="K13" s="10" t="n">
         <f aca="false">A13*J13</f>
-        <v>0.72</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1145,28 +1222,28 @@
         <v>2</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J14" s="12" t="n">
         <v>0.3</v>
@@ -1176,33 +1253,33 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
         <v>8</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J15" s="12" t="n">
         <v>0.71</v>
@@ -1212,33 +1289,33 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J16" s="12" t="n">
         <v>0.59</v>
@@ -1248,33 +1325,33 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J17" s="12" t="n">
         <v>0.94</v>
@@ -1284,33 +1361,33 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J18" s="12" t="n">
         <v>0.92</v>
@@ -1320,33 +1397,33 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J19" s="12" t="n">
         <v>0.74</v>
@@ -1356,33 +1433,33 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J20" s="15" t="n">
         <v>0.44</v>
@@ -1392,33 +1469,33 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J21" s="12" t="n">
         <v>1.36</v>
@@ -1428,7 +1505,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="n">
         <v>2</v>
       </c>
@@ -1436,25 +1513,25 @@
         <v>22</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J22" s="12" t="n">
         <v>0.1</v>
@@ -1464,33 +1541,33 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J23" s="15" t="n">
         <v>1.5</v>
@@ -1500,33 +1577,33 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J24" s="15" t="n">
         <v>4.12</v>
@@ -1536,33 +1613,33 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="J25" s="12" t="n">
         <v>1.28</v>
@@ -1577,28 +1654,28 @@
         <v>1</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="J26" s="10" t="n">
         <v>5.95</v>
@@ -1613,28 +1690,28 @@
         <v>1</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J27" s="10" t="n">
         <v>8.2</v>
@@ -1644,33 +1721,33 @@
         <v>8.2</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J28" s="10" t="n">
         <v>6.98</v>
@@ -1680,7 +1757,7 @@
         <v>6.98</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,27 +1765,29 @@
         <v>1</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>128</v>
+        <v>22</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I29" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="J29" s="10" t="n">
         <v>3</v>
       </c>
@@ -1719,7 +1798,7 @@
     </row>
     <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="19" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1729,18 +1808,18 @@
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="J30" s="21"/>
       <c r="K30" s="21" t="n">
         <f aca="false">SUM(K10:K29)</f>
-        <v>48</v>
+        <v>46.15</v>
       </c>
       <c r="L30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="19" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -1778,4 +1857,294 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="55.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="n">
+        <v>43377</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="28" t="n">
+        <f aca="false">SUMIF(D:D,D17,E:E)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="n">
+        <v>43384</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="30" t="n">
+        <f aca="false">25.96+7.99</f>
+        <v>33.95</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="28" t="n">
+        <f aca="false">SUMIF(D:D,D18,E:E)</f>
+        <v>33.95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="28" t="n">
+        <f aca="false">SUMIF(D:D,D19,E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="28" t="n">
+        <f aca="false">SUMIF(D:D,D20,E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="30" t="n">
+        <f aca="false">SUM(E2:E6)</f>
+        <v>38.95</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>